<commit_message>
Auto import assessoren finished, moving to Teamleaders import functions
</commit_message>
<xml_diff>
--- a/public/Assessor Lijst Layout.xlsx
+++ b/public/Assessor Lijst Layout.xlsx
@@ -5,15 +5,14 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mazey_000\Documents\WORK\Websites\Roctracker\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mazeyar\Desktop\School\Web\Roctracker\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Lijst" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad3" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Lijst!$A$1:$J$1</definedName>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="214">
   <si>
     <t>Naam deelnemer</t>
   </si>
@@ -655,7 +654,16 @@
     <t>Yvonne Wilbers</t>
   </si>
   <si>
-    <t>dsaasadssad</t>
+    <t>Mazeyar Rezaei</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>ja</t>
+  </si>
+  <si>
+    <t>Lisa van Dalen</t>
   </si>
 </sst>
 </file>
@@ -677,13 +685,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -708,6 +709,12 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -768,7 +775,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -806,12 +813,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -819,34 +837,34 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -855,18 +873,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -882,36 +900,36 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -923,7 +941,7 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -936,9 +954,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1247,13 +1266,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J124"/>
+  <dimension ref="A1:J126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
@@ -1265,7 +1284,7 @@
     <col min="10" max="10" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1297,7 +1316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1325,8 +1344,11 @@
       <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>18</v>
       </c>
@@ -1354,8 +1376,11 @@
       <c r="I3" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1383,8 +1408,11 @@
       <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>31</v>
       </c>
@@ -1412,8 +1440,11 @@
       <c r="I5" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>35</v>
       </c>
@@ -1441,8 +1472,11 @@
       <c r="I6" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
@@ -1470,8 +1504,11 @@
       <c r="I7" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
@@ -1499,8 +1536,11 @@
       <c r="I8" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>44</v>
       </c>
@@ -1528,8 +1568,11 @@
       <c r="I9" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J9" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>46</v>
       </c>
@@ -1557,8 +1600,11 @@
       <c r="I10" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>52</v>
       </c>
@@ -1586,8 +1632,11 @@
       <c r="I11" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>55</v>
       </c>
@@ -1615,8 +1664,11 @@
       <c r="I12" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J12" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1644,8 +1696,11 @@
       <c r="I13" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>60</v>
       </c>
@@ -1673,8 +1728,11 @@
       <c r="I14" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J14" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>62</v>
       </c>
@@ -1702,8 +1760,11 @@
       <c r="I15" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J15" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>65</v>
       </c>
@@ -1731,8 +1792,11 @@
       <c r="I16" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="23" t="s">
         <v>66</v>
       </c>
@@ -1760,8 +1824,11 @@
       <c r="I17" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>67</v>
       </c>
@@ -1789,8 +1856,11 @@
       <c r="I18" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>68</v>
       </c>
@@ -1818,8 +1888,11 @@
       <c r="I19" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>69</v>
       </c>
@@ -1847,8 +1920,11 @@
       <c r="I20" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>73</v>
       </c>
@@ -1876,8 +1952,11 @@
       <c r="I21" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
@@ -1905,8 +1984,11 @@
       <c r="I22" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>80</v>
       </c>
@@ -1934,8 +2016,11 @@
       <c r="I23" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>82</v>
       </c>
@@ -1963,8 +2048,11 @@
       <c r="I24" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>83</v>
       </c>
@@ -1992,8 +2080,11 @@
       <c r="I25" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>85</v>
       </c>
@@ -2021,8 +2112,11 @@
       <c r="I26" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>86</v>
       </c>
@@ -2050,8 +2144,11 @@
       <c r="I27" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>89</v>
       </c>
@@ -2079,8 +2176,11 @@
       <c r="I28" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>90</v>
       </c>
@@ -2108,8 +2208,11 @@
       <c r="I29" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>91</v>
       </c>
@@ -2137,8 +2240,11 @@
       <c r="I30" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>92</v>
       </c>
@@ -2166,8 +2272,11 @@
       <c r="I31" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>95</v>
       </c>
@@ -2195,8 +2304,11 @@
       <c r="I32" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>96</v>
       </c>
@@ -2224,8 +2336,11 @@
       <c r="I33" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>98</v>
       </c>
@@ -2253,8 +2368,11 @@
       <c r="I34" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>99</v>
       </c>
@@ -2282,8 +2400,11 @@
       <c r="I35" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>100</v>
       </c>
@@ -2311,8 +2432,11 @@
       <c r="I36" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>102</v>
       </c>
@@ -2340,8 +2464,11 @@
       <c r="I37" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>103</v>
       </c>
@@ -2369,8 +2496,11 @@
       <c r="I38" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>104</v>
       </c>
@@ -2398,8 +2528,11 @@
       <c r="I39" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>105</v>
       </c>
@@ -2427,8 +2560,11 @@
       <c r="I40" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>106</v>
       </c>
@@ -2456,8 +2592,11 @@
       <c r="I41" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
         <v>107</v>
       </c>
@@ -2485,8 +2624,11 @@
       <c r="I42" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>108</v>
       </c>
@@ -2514,8 +2656,11 @@
       <c r="I43" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="15" t="s">
         <v>111</v>
       </c>
@@ -2543,8 +2688,11 @@
       <c r="I44" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>112</v>
       </c>
@@ -2572,8 +2720,11 @@
       <c r="I45" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>113</v>
       </c>
@@ -2601,8 +2752,11 @@
       <c r="I46" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>114</v>
       </c>
@@ -2630,8 +2784,11 @@
       <c r="I47" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>116</v>
       </c>
@@ -2659,8 +2816,11 @@
       <c r="I48" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="15" t="s">
         <v>117</v>
       </c>
@@ -2688,8 +2848,11 @@
       <c r="I49" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>118</v>
       </c>
@@ -2717,8 +2880,11 @@
       <c r="I50" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>119</v>
       </c>
@@ -2746,8 +2912,11 @@
       <c r="I51" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="15" t="s">
         <v>121</v>
       </c>
@@ -2775,8 +2944,11 @@
       <c r="I52" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="38" t="s">
         <v>122</v>
       </c>
@@ -2804,8 +2976,11 @@
       <c r="I53" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>123</v>
       </c>
@@ -2833,8 +3008,11 @@
       <c r="I54" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>124</v>
       </c>
@@ -2862,8 +3040,11 @@
       <c r="I55" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>126</v>
       </c>
@@ -2891,8 +3072,11 @@
       <c r="I56" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>127</v>
       </c>
@@ -2920,8 +3104,11 @@
       <c r="I57" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>128</v>
       </c>
@@ -2949,8 +3136,11 @@
       <c r="I58" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>129</v>
       </c>
@@ -2978,8 +3168,11 @@
       <c r="I59" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>130</v>
       </c>
@@ -3007,8 +3200,11 @@
       <c r="I60" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>131</v>
       </c>
@@ -3036,8 +3232,11 @@
       <c r="I61" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>132</v>
       </c>
@@ -3065,8 +3264,11 @@
       <c r="I62" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>133</v>
       </c>
@@ -3094,8 +3296,11 @@
       <c r="I63" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>134</v>
       </c>
@@ -3123,8 +3328,11 @@
       <c r="I64" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>135</v>
       </c>
@@ -3152,8 +3360,11 @@
       <c r="I65" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>30</v>
       </c>
@@ -3181,8 +3392,11 @@
       <c r="I66" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
         <v>136</v>
       </c>
@@ -3210,8 +3424,11 @@
       <c r="I67" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>138</v>
       </c>
@@ -3239,8 +3456,11 @@
       <c r="I68" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>139</v>
       </c>
@@ -3268,8 +3488,11 @@
       <c r="I69" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>140</v>
       </c>
@@ -3297,8 +3520,11 @@
       <c r="I70" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J70" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>141</v>
       </c>
@@ -3326,8 +3552,11 @@
       <c r="I71" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>142</v>
       </c>
@@ -3355,8 +3584,11 @@
       <c r="I72" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>143</v>
       </c>
@@ -3384,8 +3616,11 @@
       <c r="I73" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="s">
         <v>34</v>
       </c>
@@ -3413,8 +3648,11 @@
       <c r="I74" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J74" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>145</v>
       </c>
@@ -3442,8 +3680,11 @@
       <c r="I75" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>146</v>
       </c>
@@ -3471,8 +3712,11 @@
       <c r="I76" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>147</v>
       </c>
@@ -3500,8 +3744,11 @@
       <c r="I77" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J77" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>148</v>
       </c>
@@ -3529,8 +3776,11 @@
       <c r="I78" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>150</v>
       </c>
@@ -3558,8 +3808,11 @@
       <c r="I79" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J79" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>151</v>
       </c>
@@ -3587,8 +3840,11 @@
       <c r="I80" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>152</v>
       </c>
@@ -3616,8 +3872,11 @@
       <c r="I81" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>153</v>
       </c>
@@ -3645,8 +3904,11 @@
       <c r="I82" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>154</v>
       </c>
@@ -3674,8 +3936,11 @@
       <c r="I83" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J83" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>156</v>
       </c>
@@ -3703,8 +3968,11 @@
       <c r="I84" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>158</v>
       </c>
@@ -3732,8 +4000,11 @@
       <c r="I85" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>159</v>
       </c>
@@ -3761,8 +4032,11 @@
       <c r="I86" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>160</v>
       </c>
@@ -3790,8 +4064,11 @@
       <c r="I87" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>161</v>
       </c>
@@ -3819,8 +4096,11 @@
       <c r="I88" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="23" t="s">
         <v>163</v>
       </c>
@@ -3848,8 +4128,11 @@
       <c r="I89" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>164</v>
       </c>
@@ -3877,8 +4160,11 @@
       <c r="I90" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>165</v>
       </c>
@@ -3906,8 +4192,11 @@
       <c r="I91" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>166</v>
       </c>
@@ -3935,8 +4224,11 @@
       <c r="I92" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J92" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>169</v>
       </c>
@@ -3964,8 +4256,11 @@
       <c r="I93" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>170</v>
       </c>
@@ -3993,8 +4288,11 @@
       <c r="I94" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J94" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="46" t="s">
         <v>171</v>
       </c>
@@ -4022,8 +4320,11 @@
       <c r="I95" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J95" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>172</v>
       </c>
@@ -4051,8 +4352,11 @@
       <c r="I96" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="J96" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="15" t="s">
         <v>173</v>
       </c>
@@ -4080,8 +4384,11 @@
       <c r="I97" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J97" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="15" t="s">
         <v>176</v>
       </c>
@@ -4109,8 +4416,11 @@
       <c r="I98" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J98" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="15" t="s">
         <v>178</v>
       </c>
@@ -4138,8 +4448,11 @@
       <c r="I99" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J99" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>180</v>
       </c>
@@ -4167,8 +4480,11 @@
       <c r="I100" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J100" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>181</v>
       </c>
@@ -4196,8 +4512,11 @@
       <c r="I101" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J101" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>182</v>
       </c>
@@ -4225,8 +4544,11 @@
       <c r="I102" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J102" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>183</v>
       </c>
@@ -4254,8 +4576,11 @@
       <c r="I103" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J103" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="15" t="s">
         <v>184</v>
       </c>
@@ -4283,8 +4608,11 @@
       <c r="I104" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J104" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>185</v>
       </c>
@@ -4312,8 +4640,11 @@
       <c r="I105" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J105" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>186</v>
       </c>
@@ -4341,8 +4672,11 @@
       <c r="I106" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J106" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>187</v>
       </c>
@@ -4370,8 +4704,11 @@
       <c r="I107" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J107" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>188</v>
       </c>
@@ -4399,8 +4736,11 @@
       <c r="I108" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J108" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>189</v>
       </c>
@@ -4428,8 +4768,11 @@
       <c r="I109" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J109" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>190</v>
       </c>
@@ -4457,8 +4800,11 @@
       <c r="I110" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J110" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>192</v>
       </c>
@@ -4486,8 +4832,11 @@
       <c r="I111" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J111" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>193</v>
       </c>
@@ -4515,8 +4864,11 @@
       <c r="I112" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J112" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>194</v>
       </c>
@@ -4544,8 +4896,11 @@
       <c r="I113" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J113" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>195</v>
       </c>
@@ -4573,8 +4928,11 @@
       <c r="I114" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J114" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>196</v>
       </c>
@@ -4602,8 +4960,11 @@
       <c r="I115" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J115" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>198</v>
       </c>
@@ -4631,8 +4992,11 @@
       <c r="I116" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J116" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>201</v>
       </c>
@@ -4660,8 +5024,11 @@
       <c r="I117" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J117" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>202</v>
       </c>
@@ -4689,8 +5056,11 @@
       <c r="I118" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J118" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>204</v>
       </c>
@@ -4718,8 +5088,11 @@
       <c r="I119" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J119" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" s="38" t="s">
         <v>205</v>
       </c>
@@ -4747,8 +5120,11 @@
       <c r="I120" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J120" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>206</v>
       </c>
@@ -4776,8 +5152,11 @@
       <c r="I121" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J121" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>207</v>
       </c>
@@ -4805,8 +5184,11 @@
       <c r="I122" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J122" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>208</v>
       </c>
@@ -4834,8 +5216,11 @@
       <c r="I123" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J123" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>209</v>
       </c>
@@ -4863,31 +5248,70 @@
       <c r="I124" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="J124" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C125" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D125" s="5">
+        <v>35675</v>
+      </c>
+      <c r="E125" s="6"/>
+      <c r="F125" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H125" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="I125" s="4"/>
+      <c r="J125" s="51" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A126" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C126" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D126" s="5">
+        <v>35675</v>
+      </c>
+      <c r="E126" s="6"/>
+      <c r="F126" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G126" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H126" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="I126" s="4"/>
+      <c r="J126" s="51" t="s">
+        <v>212</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A1:J1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="10" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>